<commit_message>
Se agrega informe de avances
</commit_message>
<xml_diff>
--- a/Reto pruebas manuales/Informe de defectos.xlsx
+++ b/Reto pruebas manuales/Informe de defectos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunez\Escritorio\Reto pruebas manuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB921A80-5B31-4953-9606-B55B800CBDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5728E2-D112-42BA-A43A-A42A7BEA791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>INFORME DE DEFECTOS</t>
   </si>
@@ -144,38 +144,57 @@
     <t>Servicio de numeros a dólar</t>
   </si>
   <si>
+    <t>se espera que arroje un error diciendo que no puede operar con numeros negativos y retorne un status 400</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 OK                                &lt;m:NumberToDollarsResult&gt;number too large dollars and number too large cents&lt;/m:NumberToDollarsResult&gt;</t>
+  </si>
+  <si>
+    <t>No retorna ningun valor cuando se inserta el numero 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se espera que retorne "zero dollars" y un status 200 </t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 OK                    &lt;m:NumberToDollarsResult&gt;&lt;/m:NumberToDollarsResult&gt;</t>
+  </si>
+  <si>
+    <t>No genera errores cuando no se inserta ningun valor</t>
+  </si>
+  <si>
+    <t>Se espera que genere un error ya que no se esta especificando ningun valor y generar un status 400</t>
+  </si>
+  <si>
+    <t>No genera errores cuando se ingresan valores invalidos</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>Se espera que genere un error ya que no se esta especificando ningun valor valido y generar un status 400</t>
+  </si>
+  <si>
+    <t>BUG05</t>
+  </si>
+  <si>
+    <t>No genera errores cuando no se inserta ningun texto en el conversor</t>
+  </si>
+  <si>
+    <t>Servicio de formateo de textos</t>
+  </si>
+  <si>
     <t>1. Abrir el navegador                                                        2. Buscar la plataforma dataacces.com                                                   3. Seleccionar la peticion                                                  4. Abrir SoapUI                                                   
-5. Crear un nuevo proyecto soap                                                    6.Se inserta la url del servicio seleccionado                                                                               7. Se busca el campo para ingresar el numero que se convertira                                                                           8. Se ingresa el numero a convertir                                                                9. Se oprime el boton enviar petecion                                      10. Se ejecuta la peticion</t>
-  </si>
-  <si>
-    <t>se espera que arroje un error diciendo que no puede operar con numeros negativos y retorne un status 400</t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 OK                                &lt;m:NumberToDollarsResult&gt;number too large dollars and number too large cents&lt;/m:NumberToDollarsResult&gt;</t>
-  </si>
-  <si>
-    <t>No retorna ningun valor cuando se inserta el numero 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se espera que retorne "zero dollars" y un status 200 </t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 OK                    &lt;m:NumberToDollarsResult&gt;&lt;/m:NumberToDollarsResult&gt;</t>
-  </si>
-  <si>
-    <t>No genera errores cuando no se inserta ningun valor</t>
-  </si>
-  <si>
-    <t>Se espera que genere un error ya que no se esta especificando ningun valor y generar un status 400</t>
-  </si>
-  <si>
-    <t>No genera errores cuando se ingresan valores invalidos</t>
-  </si>
-  <si>
-    <t>hola</t>
-  </si>
-  <si>
-    <t>Se espera que genere un error ya que no se esta especificando ningun valor valido y generar un status 400</t>
+5. Crear un nuevo proyecto soap                                                    6.Se inserta la url del servicio seleccionado                                                                               7. Se busca el campo para ingresar el texto que sera formateado                                                                          8. Se ingresa el texto a formatear                                                                9. Se oprime el boton enviar peticion                                      10. Se ejecuta la peticion</t>
+  </si>
+  <si>
+    <t>1. Abrir el navegador                                                        2. Buscar la plataforma dataacces.com                                                   3. Seleccionar la peticion                                                  4. Abrir SoapUI                                                   
+5. Crear un nuevo proyecto soap                                                    6.Se inserta la url del servicio seleccionado                                                                               7. Se busca el campo para ingresar el numero que se convertira                                                                           8. Se ingresa el numero a convertir                                                                9. Se oprime el boton enviar peticion                                      10. Se ejecuta la peticion</t>
+  </si>
+  <si>
+    <t>Se espera que genere un error ya que no se esta especificando ningun texto para su conversion y generar un status 400</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 OK                    &lt;m:TitleCaseWordsWithTokenResult&gt;&lt;/m:TitleCaseWordsWithTokenResult&gt;</t>
   </si>
 </sst>
 </file>
@@ -380,6 +399,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,12 +416,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +634,7 @@
   <dimension ref="A1:AE998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -638,24 +657,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="42.75" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:31" ht="29.25" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -729,20 +748,20 @@
       <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>39</v>
+      <c r="H3" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="20">
         <v>-450</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -777,7 +796,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5">
         <v>44990</v>
@@ -794,8 +813,8 @@
       <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>39</v>
+      <c r="H4" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>20</v>
@@ -804,10 +823,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="M4" s="4">
         <v>2</v>
@@ -827,7 +846,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5">
         <v>44991</v>
@@ -844,18 +863,18 @@
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>39</v>
+      <c r="H5" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" s="4">
         <v>3</v>
@@ -875,7 +894,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5">
         <v>44992</v>
@@ -892,20 +911,20 @@
       <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="24" t="s">
-        <v>39</v>
+      <c r="H6" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="L6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
@@ -920,13 +939,60 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:31" ht="158.4">
+      <c r="A7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5">
+        <v>44992</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="6">
+        <v>2</v>
+      </c>
+      <c r="N7" s="6">
+        <v>2</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:31" ht="14.25" customHeight="1">
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -973,10 +1039,10 @@
     </row>
     <row r="14" spans="1:31" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:31" ht="14.25" customHeight="1">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1025,10 +1091,10 @@
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="3:7" ht="14.25" customHeight="1">
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>

</xml_diff>